<commit_message>
changed the testdata excel file
</commit_message>
<xml_diff>
--- a/testData/ReadAndWriteData.xlsx
+++ b/testData/ReadAndWriteData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408449\git\hackthonV1\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2408309_cognizant_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0BBBA3-D286-4678-843B-E9C5BC1BF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{6E0BBBA3-D286-4678-843B-E9C5BC1BF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1CE9C65-3B67-460F-BDB3-22EA76F78D15}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E95DD8B-A033-481F-88F3-D6F98D7B15B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7E95DD8B-A033-481F-88F3-D6F98D7B15B9}"/>
   </bookViews>
   <sheets>
     <sheet name="TopCities" sheetId="1" r:id="rId1"/>
@@ -38,38 +38,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
-  <si>
-    <t>rohan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>as</t>
   </si>
   <si>
-    <t>rohan@gmail.com</t>
-  </si>
-  <si>
     <t>&lt;500</t>
   </si>
   <si>
     <t>Taking a demo</t>
   </si>
   <si>
-    <t>siva</t>
-  </si>
-  <si>
     <t xml:space="preserve">as </t>
   </si>
   <si>
-    <t>siva@gmail.com</t>
-  </si>
-  <si>
-    <t>krihsna</t>
-  </si>
-  <si>
-    <t>krishna</t>
-  </si>
-  <si>
     <t>Bangalore</t>
   </si>
   <si>
@@ -122,6 +104,30 @@
   </si>
   <si>
     <t>Validation is triggered on entering an invalid input</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>Hada</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>akashsingh.4111@gmail.com</t>
+  </si>
+  <si>
+    <t>hada@gmail.com</t>
+  </si>
+  <si>
+    <t>sharma</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Manipal Hospital Varthur Road (formerly Columbia Asia Hospital)</t>
   </si>
 </sst>
 </file>
@@ -525,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9E61B5-D6CB-4812-9DC5-28D8ACD14421}">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B2:B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,44 +544,44 @@
     <row r="2" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s" s="0">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s" s="0">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="0">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -587,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED943D8-72C4-441D-B9F0-E524BE35F9EB}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,76 +603,76 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" s="0">
+        <v>8317096478</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" s="0">
-        <v>9108716657</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="G1" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s" s="0">
+      <c r="C2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0">
-        <v>812321</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
         <v>9108223242</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
     </row>
   </sheetData>
@@ -680,57 +686,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:B9"/>
+  <dimension ref="B1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="B1:C11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s" s="0">
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="s" s="0">
+    <row r="10">
+      <c r="B10" t="s" s="0">
         <v>19</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="0">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>